<commit_message>
Update Detention hearing outcomes.xlsx
</commit_message>
<xml_diff>
--- a/Detention hearing outcomes.xlsx
+++ b/Detention hearing outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dstemen\Documents\GitHub\CCJ.Illinois\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BD55B2A-F159-4730-851E-B186BC7B2E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3875D61E-63DE-40B6-9A91-4F0220D0E8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="16545" windowHeight="9570" xr2:uid="{BD2D69C5-1F00-47BB-851E-7E456156F599}"/>
   </bookViews>
@@ -86,9 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F918CC-0144-491B-8610-D407F1C06CC0}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -427,13 +425,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>29</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>60</v>
       </c>
       <c r="D2">
@@ -441,22 +439,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>71</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>40</v>
       </c>
       <c r="D3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>